<commit_message>
Excel calculator manual experiments
</commit_message>
<xml_diff>
--- a/keys_calculator.xlsx
+++ b/keys_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Fog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F67F3D8-A41F-4C49-A686-31B5A6020853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEBE214-1F68-46EA-8488-98AECECEA848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="1305" windowWidth="19410" windowHeight="13950" xr2:uid="{2E81292D-3F82-4C88-9AC7-2643B8815C89}"/>
+    <workbookView xWindow="7830" yWindow="2415" windowWidth="19410" windowHeight="13950" xr2:uid="{2E81292D-3F82-4C88-9AC7-2643B8815C89}"/>
   </bookViews>
   <sheets>
     <sheet name="Fog keys calculator" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Индекс</t>
   </si>
@@ -36,16 +36,13 @@
     <t>Первичный ключ</t>
   </si>
   <si>
-    <t>Исходный ключ</t>
-  </si>
-  <si>
     <t>XOR ключ</t>
   </si>
   <si>
     <t>Ключ сдвига</t>
   </si>
   <si>
-    <t>Контрольное число XOR ключа</t>
+    <t>Контрольное число текущего XOR ключа</t>
   </si>
 </sst>
 </file>
@@ -104,23 +101,40 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -143,37 +157,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,127 +555,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8439D1-314C-4BBB-B049-F0234957BFD3}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="13" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="13" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
     <row r="2" spans="1:14" ht="17.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>4</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>6</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>7</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>8</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <v>9</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>10</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <v>11</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <v>12</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="17.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="E3" s="11">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="H3" s="11">
         <v>2</v>
       </c>
-      <c r="D3" s="8">
+      <c r="I3" s="11">
         <v>3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="J3" s="11">
         <v>4</v>
       </c>
-      <c r="F3" s="8">
+      <c r="K3" s="11">
         <v>5</v>
       </c>
-      <c r="G3" s="8">
+      <c r="L3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="M3" s="11">
         <v>2</v>
       </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="8">
-        <v>4</v>
-      </c>
-      <c r="K3" s="8">
-        <v>5</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8">
-        <v>2</v>
-      </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" ht="15.75">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9">
         <f>POWER(B3,2)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="10">
         <f>C3+C2*10</f>
         <v>22</v>
       </c>
@@ -618,7 +668,7 @@
         <f>POWER(D3,2)</f>
         <v>9</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="10">
         <f>E3+E2*10</f>
         <v>44</v>
       </c>
@@ -626,7 +676,7 @@
         <f>POWER(F3,2)</f>
         <v>25</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="10">
         <f>G3+G2*10</f>
         <v>61</v>
       </c>
@@ -634,7 +684,7 @@
         <f>POWER(H3,2)</f>
         <v>4</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="10">
         <f>I3+I2*10</f>
         <v>83</v>
       </c>
@@ -642,7 +692,7 @@
         <f>POWER(J3,2)</f>
         <v>16</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="10">
         <f>K3+K2*10</f>
         <v>105</v>
       </c>
@@ -650,15 +700,15 @@
         <f>POWER(L3,2)</f>
         <v>1</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="10">
         <f>M3+M2*10</f>
         <v>122</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
+      <c r="A5" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B5" s="9">
         <f>_xlfn.BITXOR(B2,B4)</f>
@@ -710,109 +760,94 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
-        <f>B5+B4+$B$8</f>
-        <v>12</v>
-      </c>
-      <c r="C6" s="9">
-        <f>C5+C4-$B$8</f>
-        <v>31</v>
-      </c>
-      <c r="D6" s="9">
-        <f>D5+D4+$B$8</f>
-        <v>30</v>
-      </c>
-      <c r="E6" s="9">
-        <f>E5+E4-$B$8</f>
-        <v>73</v>
-      </c>
-      <c r="F6" s="9">
-        <f>F5+F4+$B$8</f>
-        <v>64</v>
-      </c>
-      <c r="G6" s="9">
-        <f>G5+G4-$B$8</f>
-        <v>109</v>
-      </c>
-      <c r="H6" s="9">
-        <f>H5+H4+$B$8</f>
-        <v>18</v>
-      </c>
-      <c r="I6" s="9">
-        <f>I5+I4-$B$8</f>
-        <v>163</v>
-      </c>
-      <c r="J6" s="9">
-        <f>J5+J4+$B$8</f>
-        <v>52</v>
-      </c>
-      <c r="K6" s="9">
-        <f>K5+K4-$B$8</f>
-        <v>193</v>
-      </c>
-      <c r="L6" s="9">
-        <f>L5+L4+$B$8</f>
-        <v>22</v>
-      </c>
-      <c r="M6" s="9">
-        <f>M5+M4-$B$8</f>
-        <v>229</v>
-      </c>
-      <c r="N6" s="5"/>
+      <c r="B6" s="12">
+        <f>MOD(SUM(B5:M5),12)</f>
+        <v>11</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <f>IF(B5&gt;1000,LEFT(B5,3)+B2,B5)+$B$6</f>
+        <v>11</v>
+      </c>
+      <c r="C7" s="15">
+        <f>IF(C5&gt;1000,LEFT(C5,3)+C2,C5)-$B$6</f>
+        <v>9</v>
+      </c>
+      <c r="D7" s="15">
+        <f>IF(D5&gt;1000,LEFT(D5,3)+D2,D5)+$B$6</f>
+        <v>21</v>
+      </c>
+      <c r="E7" s="15">
+        <f>IF(E5&gt;1000,LEFT(E5,3)+E2,E5)-$B$6</f>
+        <v>29</v>
+      </c>
+      <c r="F7" s="15">
+        <f>IF(F5&gt;1000,LEFT(F5,3)+F2,F5)+$B$6</f>
+        <v>39</v>
+      </c>
+      <c r="G7" s="15">
+        <f>IF(G5&gt;1000,LEFT(G5,3)+G2,G5)-$B$6</f>
+        <v>48</v>
+      </c>
+      <c r="H7" s="15">
+        <f>IF(H5&gt;1000,LEFT(H5,3)+H2,H5)+$B$6</f>
+        <v>14</v>
+      </c>
+      <c r="I7" s="15">
+        <f>IF(I5&gt;1000,LEFT(I5,3)+I2,I5)-$B$6</f>
+        <v>80</v>
+      </c>
+      <c r="J7" s="15">
+        <f>IF(J5&gt;1000,LEFT(J5,3)+J2,J5)+$B$6</f>
+        <v>36</v>
+      </c>
+      <c r="K7" s="15">
+        <f>IF(K5&gt;1000,LEFT(K5,3)+K2,K5)-$B$6</f>
+        <v>88</v>
+      </c>
+      <c r="L7" s="15">
+        <f>IF(L5&gt;1000,LEFT(L5,3)+L2,L5)+$B$6</f>
+        <v>21</v>
+      </c>
+      <c r="M7" s="15">
+        <f>IF(M5&gt;1000,LEFT(M5,3)+M2,M5)-$B$6</f>
+        <v>107</v>
+      </c>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11">
-        <f>MOD(SUM(B5:M5),12)</f>
-        <v>11</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="A8" s="8"/>
+      <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>12345</v>
-      </c>
+    <row r="15" spans="1:14">
+      <c r="D15" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:M6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C4 E4 G4 I4 K4 C6 E6 G6 I6 K6" formula="1"/>
+    <ignoredError sqref="E4 G4 I4 K4" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>